<commit_message>
cambios en el historial del paciente
</commit_message>
<xml_diff>
--- a/SistemaMedico/Recetas.xlsx
+++ b/SistemaMedico/Recetas.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+  <si>
+    <t>ID receta</t>
   </si>
   <si>
     <t>Paciente</t>
@@ -29,15 +29,48 @@
     <t>Fecha Emisión</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>dolocloralan</t>
+  </si>
+  <si>
+    <t>2025-10-24 10:27</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Bactrim</t>
+  </si>
+  <si>
+    <t>2025-10-24 10:12</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Migradol cada 8 horas</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
     <t>Ana</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Pomada</t>
   </si>
   <si>
@@ -45,9 +78,6 @@
   </si>
   <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>José</t>
   </si>
   <si>
     <t>Antiflamatorio 100ml</t>
@@ -107,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -155,30 +185,81 @@
         <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="0">
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>16</v>
+      <c r="C6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>